<commit_message>
metiendo todo en el excel funcionando con funcion
</commit_message>
<xml_diff>
--- a/MSExcel_In_Java-master/datos_procesados.xlsx
+++ b/MSExcel_In_Java-master/datos_procesados.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ETQ</t>
   </si>
@@ -27,6 +27,12 @@
   </si>
   <si>
     <t>SIZE</t>
+  </si>
+  <si>
+    <t>ORG</t>
+  </si>
+  <si>
+    <t>%00001111</t>
   </si>
   <si>
     <t>Et1</t>
@@ -45,6 +51,18 @@
   </si>
   <si>
     <t>@4732</t>
+  </si>
+  <si>
+    <t>SWI</t>
+  </si>
+  <si>
+    <t>DS.B</t>
+  </si>
+  <si>
+    <t>%0011000011111100</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
@@ -89,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -112,27 +130,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="3">
+      <c r="A3"/>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>